<commit_message>
agregando categoria en productos
</commit_message>
<xml_diff>
--- a/modelado/Diccionario_Datos_ERP_Pricing.xlsx
+++ b/modelado/Diccionario_Datos_ERP_Pricing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\erp2027\modelado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEA6A3D-BCCB-4FA5-B599-82C7CDBA2C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9120D1F0-5F1D-44F6-A2C8-C7BA0C7F8EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="2025" windowWidth="23730" windowHeight="14175" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="INDEX" sheetId="1" r:id="rId1"/>
@@ -679,14 +679,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="17.28515625" customWidth="1"/>
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -857,6 +860,11 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>